<commit_message>
Reworked Query 5 section. Added new scatter plots
</commit_message>
<xml_diff>
--- a/project_sql/Data Analyses/5_optimal_skills_insights.xlsx
+++ b/project_sql/Data Analyses/5_optimal_skills_insights.xlsx
@@ -5,18 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blnor\Downloads\Brennan\SQL for Data Analytics\SQL_Project_Data_Job_Analysis\project_sql\Data Analyses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blnor\Downloads\Brennan\Online Classes and Projects\SQL for Data Analytics\SQL_Project_Data_Job_Analysis\project_sql\Data Analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6D4462-3C24-4A7F-A235-E0EF719CDE81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41B0BBE-BAA7-4BFE-B1A5-5EB34A522D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RAW_DATA" sheetId="1" r:id="rId1"/>
     <sheet name="Scatter Plot" sheetId="4" r:id="rId2"/>
     <sheet name="Insights" sheetId="2" r:id="rId3"/>
     <sheet name="Pareto Charts" sheetId="3" r:id="rId4"/>
+    <sheet name="RAW_DATA - Salary Prio" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'Pareto Charts'!$A$2:$A$26</definedName>
@@ -24,11 +25,6 @@
     <definedName name="_xlchart.v1.2" hidden="1">'Pareto Charts'!$B$2:$B$26</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">'Pareto Charts'!$C$1</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">'Pareto Charts'!$C$2:$C$26</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Pareto Charts'!$A$2:$A$26</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Pareto Charts'!$B$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Pareto Charts'!$B$2:$B$26</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Pareto Charts'!$C$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'Pareto Charts'!$C$2:$C$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="56">
   <si>
     <t>sql</t>
   </si>
@@ -165,6 +161,60 @@
   </si>
   <si>
     <t>Average Rank</t>
+  </si>
+  <si>
+    <t>skills</t>
+  </si>
+  <si>
+    <t>demand_count</t>
+  </si>
+  <si>
+    <t>average_salary</t>
+  </si>
+  <si>
+    <t>Go</t>
+  </si>
+  <si>
+    <t>Confluence</t>
+  </si>
+  <si>
+    <t>Hadoop</t>
+  </si>
+  <si>
+    <t>Snowflake</t>
+  </si>
+  <si>
+    <t>Azure</t>
+  </si>
+  <si>
+    <t>Bigquery</t>
+  </si>
+  <si>
+    <t>Aws</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>Ssis</t>
+  </si>
+  <si>
+    <t>Jira</t>
+  </si>
+  <si>
+    <t>Oracle</t>
+  </si>
+  <si>
+    <t>Looker</t>
+  </si>
+  <si>
+    <t>Nosql</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -529,7 +579,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -564,6 +614,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -2451,6 +2502,1187 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Salary VS</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Demand - Salary Prioritized</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'RAW_DATA - Salary Prio'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>average_salary</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{98C63819-9026-4AFF-92AF-F84E0784B67E}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-7714-45C6-B6AB-76AEFFD78921}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{A0CDC1A6-748D-4541-BD14-615FC65DDABA}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-7714-45C6-B6AB-76AEFFD78921}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{1ABDFED7-63F0-4AB1-A514-A795BA4E6D9D}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-7714-45C6-B6AB-76AEFFD78921}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{900D1FB0-67EA-4798-968D-787846E0E06D}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-7714-45C6-B6AB-76AEFFD78921}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{08AAFB6A-DA51-4A0F-B46D-3EBBA614B15E}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-7714-45C6-B6AB-76AEFFD78921}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{698EE087-4783-4F88-B5C7-7DFCE368AE05}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-7714-45C6-B6AB-76AEFFD78921}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{948AAB4B-FA4E-4475-AB13-DAD85285B572}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-7714-45C6-B6AB-76AEFFD78921}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{5E661292-B781-490E-9E81-EC72465098EB}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-7714-45C6-B6AB-76AEFFD78921}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{B65C8B35-8704-4589-B54B-4219F19A2132}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-7714-45C6-B6AB-76AEFFD78921}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{1CE4B4A9-08FE-4B30-BCA9-BFD1C56C9739}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-7714-45C6-B6AB-76AEFFD78921}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{72552C1F-8615-4E9D-9F08-67FF940B87E5}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-7714-45C6-B6AB-76AEFFD78921}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{3F1324A3-EDAE-47D3-8917-59332A333E18}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-7714-45C6-B6AB-76AEFFD78921}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{C8A80696-EBDE-465C-B659-E26864B906B0}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000D-7714-45C6-B6AB-76AEFFD78921}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{49BC4B07-05F7-4289-92DC-9A51E5215475}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000E-7714-45C6-B6AB-76AEFFD78921}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{33F5A35E-282A-4F4F-A3D4-2294F7E5737A}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-7714-45C6-B6AB-76AEFFD78921}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'RAW_DATA - Salary Prio'!$B$2:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>148</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'RAW_DATA - Salary Prio'!$C$2:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>115320</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>114210</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>113193</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>112948</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>111225</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>109654</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>108317</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>106906</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>106683</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>104918</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>104534</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>103795</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>101414</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>101397</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100499</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>'RAW_DATA - Salary Prio'!$A$2:$A$16</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="15"/>
+                  <c:pt idx="0">
+                    <c:v>Go</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Confluence</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Hadoop</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Snowflake</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Azure</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Bigquery</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Aws</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Java</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Ssis</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Jira</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Oracle</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Looker</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Nosql</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Python</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>R</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7714-45C6-B6AB-76AEFFD78921}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1628787072"/>
+        <c:axId val="1628784672"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1628787072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Demand</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1628784672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1628784672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Salary</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1628787072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
@@ -2722,6 +3954,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
   <cs:axisTitle>
@@ -4759,6 +6031,508 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
@@ -5249,6 +7023,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>504823</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>52385</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>523874</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{833BF315-E6A8-AEFF-EAC3-4AA614386CE6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6872,7 +8687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{974B111E-8F87-49DA-8A3B-27CDDF919008}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Y41" sqref="Y41"/>
     </sheetView>
   </sheetViews>
@@ -7359,4 +9174,201 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{898A4D4B-A621-4305-B695-94411F426BDA}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2">
+        <v>27</v>
+      </c>
+      <c r="C2" s="34">
+        <v>115320</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3">
+        <v>11</v>
+      </c>
+      <c r="C3" s="34">
+        <v>114210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4">
+        <v>22</v>
+      </c>
+      <c r="C4" s="34">
+        <v>113193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5">
+        <v>37</v>
+      </c>
+      <c r="C5" s="34">
+        <v>112948</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6">
+        <v>34</v>
+      </c>
+      <c r="C6" s="34">
+        <v>111225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7">
+        <v>13</v>
+      </c>
+      <c r="C7" s="34">
+        <v>109654</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8">
+        <v>32</v>
+      </c>
+      <c r="C8" s="34">
+        <v>108317</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9">
+        <v>17</v>
+      </c>
+      <c r="C9" s="34">
+        <v>106906</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10">
+        <v>12</v>
+      </c>
+      <c r="C10" s="34">
+        <v>106683</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+      <c r="C11" s="34">
+        <v>104918</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12">
+        <v>37</v>
+      </c>
+      <c r="C12" s="34">
+        <v>104534</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13">
+        <v>49</v>
+      </c>
+      <c r="C13" s="34">
+        <v>103795</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" s="34">
+        <v>101414</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15">
+        <v>236</v>
+      </c>
+      <c r="C15" s="34">
+        <v>101397</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16">
+        <v>148</v>
+      </c>
+      <c r="C16" s="34">
+        <v>100499</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>